<commit_message>
update curve log and add measurements from 4/23
</commit_message>
<xml_diff>
--- a/data_log_sheets/TT24_curve_log.xlsx
+++ b/data_log_sheets/TT24_curve_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data_log_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3D7CF4-6C8F-6447-9CE9-6C02355CA5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D06FC3D-1C55-3F41-B7B7-CDAF2A75FA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="500" windowWidth="37800" windowHeight="28300" xr2:uid="{A62C6EB1-ACA7-F14B-BE94-73C128140FF4}"/>
+    <workbookView xWindow="3400" yWindow="500" windowWidth="37800" windowHeight="28300" xr2:uid="{A62C6EB1-ACA7-F14B-BE94-73C128140FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="26">
   <si>
     <t>date</t>
   </si>
@@ -87,6 +87,33 @@
   </si>
   <si>
     <t>closest to fence</t>
+  </si>
+  <si>
+    <t>striped2</t>
+  </si>
+  <si>
+    <t>right at plot mid-point</t>
+  </si>
+  <si>
+    <t>notebook fell onto individual. Curve present but no carbon budget for ind</t>
+  </si>
+  <si>
+    <t>second striped flag away from fence</t>
+  </si>
+  <si>
+    <t>LI-6800 died before getting to plant. Second log file noted with "_b" suffix</t>
+  </si>
+  <si>
+    <t>flag8</t>
+  </si>
+  <si>
+    <t>curve_fit</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -94,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -129,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,19 +491,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD84A7C-B77D-134C-A552-72D1D4E0C426}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="286" zoomScaleNormal="286" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="286" zoomScaleNormal="286" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="59.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,11 +523,14 @@
       <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45395</v>
       </c>
@@ -518,11 +549,14 @@
       <c r="F2" s="3">
         <v>7.4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45395</v>
       </c>
@@ -541,8 +575,11 @@
       <c r="F3" s="3">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45395</v>
       </c>
@@ -561,8 +598,11 @@
       <c r="F4" s="3">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45395</v>
       </c>
@@ -581,8 +621,11 @@
       <c r="F5" s="3">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45395</v>
       </c>
@@ -601,11 +644,14 @@
       <c r="F6" s="3">
         <v>6.8</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45395</v>
       </c>
@@ -624,11 +670,14 @@
       <c r="F7" s="3">
         <v>6.4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45395</v>
       </c>
@@ -647,8 +696,11 @@
       <c r="F8" s="3">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45395</v>
       </c>
@@ -667,8 +719,11 @@
       <c r="F9" s="3">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45395</v>
       </c>
@@ -687,8 +742,11 @@
       <c r="F10" s="3">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45395</v>
       </c>
@@ -707,8 +765,11 @@
       <c r="F11" s="3">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45395</v>
       </c>
@@ -727,8 +788,11 @@
       <c r="F12" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45395</v>
       </c>
@@ -747,8 +811,11 @@
       <c r="F13" s="3">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45395</v>
       </c>
@@ -767,8 +834,11 @@
       <c r="F14" s="3">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45395</v>
       </c>
@@ -787,8 +857,11 @@
       <c r="F15" s="3">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45395</v>
       </c>
@@ -807,11 +880,14 @@
       <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>45395</v>
       </c>
@@ -830,8 +906,11 @@
       <c r="F17" s="3">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45395</v>
       </c>
@@ -850,8 +929,11 @@
       <c r="F18" s="3">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>45395</v>
       </c>
@@ -870,8 +952,11 @@
       <c r="F19" s="3">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>45396</v>
       </c>
@@ -890,8 +975,11 @@
       <c r="F20" s="3">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>45396</v>
       </c>
@@ -910,8 +998,11 @@
       <c r="F21" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>45396</v>
       </c>
@@ -930,8 +1021,11 @@
       <c r="F22" s="3">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>45396</v>
       </c>
@@ -950,8 +1044,11 @@
       <c r="F23" s="3">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>45396</v>
       </c>
@@ -970,11 +1067,14 @@
       <c r="F24" s="3">
         <v>7.5</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>45396</v>
       </c>
@@ -993,8 +1093,11 @@
       <c r="F25" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>45396</v>
       </c>
@@ -1013,8 +1116,11 @@
       <c r="F26" s="3">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>45396</v>
       </c>
@@ -1033,8 +1139,11 @@
       <c r="F27" s="3">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>45396</v>
       </c>
@@ -1053,8 +1162,11 @@
       <c r="F28" s="3">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>45396</v>
       </c>
@@ -1073,8 +1185,11 @@
       <c r="F29" s="3">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>45396</v>
       </c>
@@ -1093,8 +1208,11 @@
       <c r="F30" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>45396</v>
       </c>
@@ -1113,8 +1231,11 @@
       <c r="F31" s="3">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>45396</v>
       </c>
@@ -1133,8 +1254,11 @@
       <c r="F32" s="3">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45396</v>
       </c>
@@ -1153,8 +1277,11 @@
       <c r="F33" s="3">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45396</v>
       </c>
@@ -1173,8 +1300,11 @@
       <c r="F34" s="3">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45396</v>
       </c>
@@ -1193,8 +1323,11 @@
       <c r="F35" s="3">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45396</v>
       </c>
@@ -1213,8 +1346,11 @@
       <c r="F36" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>45397</v>
       </c>
@@ -1233,8 +1369,11 @@
       <c r="F37" s="3">
         <v>10.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45397</v>
       </c>
@@ -1253,8 +1392,11 @@
       <c r="F38" s="3">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45397</v>
       </c>
@@ -1273,8 +1415,11 @@
       <c r="F39" s="3">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45397</v>
       </c>
@@ -1293,11 +1438,14 @@
       <c r="F40" s="3">
         <v>6.8</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>45397</v>
       </c>
@@ -1316,8 +1464,11 @@
       <c r="F41" s="3">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45397</v>
       </c>
@@ -1336,8 +1487,11 @@
       <c r="F42" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45397</v>
       </c>
@@ -1356,8 +1510,11 @@
       <c r="F43" s="3">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45397</v>
       </c>
@@ -1376,11 +1533,14 @@
       <c r="F44" s="3">
         <v>10.5</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45397</v>
       </c>
@@ -1399,8 +1559,11 @@
       <c r="F45" s="3">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45397</v>
       </c>
@@ -1419,8 +1582,11 @@
       <c r="F46" s="3">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45397</v>
       </c>
@@ -1439,8 +1605,11 @@
       <c r="F47" s="3">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45397</v>
       </c>
@@ -1459,11 +1628,14 @@
       <c r="F48" s="3">
         <v>8.1</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45397</v>
       </c>
@@ -1482,8 +1654,11 @@
       <c r="F49" s="3">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45397</v>
       </c>
@@ -1502,8 +1677,11 @@
       <c r="F50" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>45397</v>
       </c>
@@ -1521,6 +1699,780 @@
       </c>
       <c r="F51" s="3">
         <v>9</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>5060</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="F52" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>5783</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="F53" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>5031</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F54" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55">
+        <v>4543</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="F55" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>2276</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>4511</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="F57" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+      <c r="C58">
+        <v>3770</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="F58" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <v>4582</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="F59" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="C60">
+        <v>2980</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="F60" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+      <c r="C61">
+        <v>3371</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.53263888888888888</v>
+      </c>
+      <c r="F61" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>3379</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="F62" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>4505</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="F63" s="3">
+        <v>12</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>4745</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="F64" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>5722</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F65" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>2921</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F66" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0.59652777777777777</v>
+      </c>
+      <c r="F67" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>5642</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F68" s="3">
+        <v>9.9</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B69">
+        <v>6</v>
+      </c>
+      <c r="C69">
+        <v>6879</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="F69" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>7120</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0.43680555555555556</v>
+      </c>
+      <c r="F70" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>2912</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="F71" s="3">
+        <v>13</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B72">
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <v>614</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0.46041666666666664</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B73">
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <v>1374</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="F73" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B74">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>6881</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="2">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="F74" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>5381</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="F75" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>4105</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="F76" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>4547</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="2">
+        <v>0.51388888888888884</v>
+      </c>
+      <c r="F77" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78">
+        <v>2388</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="F78" s="3">
+        <v>14.3</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>5904</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="2">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="F79" s="3">
+        <v>11</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80">
+        <v>7147</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="2">
+        <v>0.54513888888888884</v>
+      </c>
+      <c r="F80" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>43</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="2">
+        <v>0.51388888888888884</v>
+      </c>
+      <c r="F81" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82">
+        <v>83</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="F82" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>22</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="F83" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <v>2563</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="2">
+        <v>0.5854166666666667</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add curve fits from second week
</commit_message>
<xml_diff>
--- a/data_log_sheets/TT24_curve_log.xlsx
+++ b/data_log_sheets/TT24_curve_log.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data_log_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D06FC3D-1C55-3F41-B7B7-CDAF2A75FA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1FB14C-12AF-C843-B2E3-A2801931BD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="500" windowWidth="37800" windowHeight="28300" xr2:uid="{A62C6EB1-ACA7-F14B-BE94-73C128140FF4}"/>
+    <workbookView minimized="1" xWindow="13400" yWindow="500" windowWidth="37800" windowHeight="28300" xr2:uid="{A62C6EB1-ACA7-F14B-BE94-73C128140FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="29">
   <si>
     <t>date</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>flag3</t>
+  </si>
+  <si>
+    <t>flag1</t>
+  </si>
+  <si>
+    <t>flag2</t>
   </si>
 </sst>
 </file>
@@ -491,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD84A7C-B77D-134C-A552-72D1D4E0C426}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="286" zoomScaleNormal="286" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="286" zoomScaleNormal="286" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1724,7 +1733,7 @@
         <v>10.3</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1747,7 +1756,7 @@
         <v>10.6</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1770,7 +1779,7 @@
         <v>9.4</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1793,7 +1802,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H55" t="s">
         <v>18</v>
@@ -1819,7 +1828,7 @@
         <v>6.8</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -1842,7 +1851,7 @@
         <v>11.6</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -1865,7 +1874,7 @@
         <v>8.1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H58" t="s">
         <v>19</v>
@@ -1891,7 +1900,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -1914,7 +1923,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1937,7 +1946,7 @@
         <v>11.2</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -1960,7 +1969,7 @@
         <v>6.2</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -1983,7 +1992,7 @@
         <v>12</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2006,7 +2015,7 @@
         <v>13.1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2029,7 +2038,7 @@
         <v>13.2</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2052,7 +2061,7 @@
         <v>11.1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2075,7 +2084,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H67" t="s">
         <v>20</v>
@@ -2101,7 +2110,7 @@
         <v>9.9</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2124,7 +2133,7 @@
         <v>10.3</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H69" t="s">
         <v>21</v>
@@ -2472,6 +2481,236 @@
         <v>8</v>
       </c>
       <c r="G84" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+      <c r="C85">
+        <v>4265</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F85" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>2573</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F86" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87">
+        <v>2547</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F87" s="3">
+        <v>14</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+      <c r="C88">
+        <v>4177</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="F88" s="3">
+        <v>15</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B89">
+        <v>5</v>
+      </c>
+      <c r="C89">
+        <v>1795</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F89" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="C90" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F90" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F91" s="3">
+        <v>12</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B92">
+        <v>5</v>
+      </c>
+      <c r="C92" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="F92" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B93">
+        <v>5</v>
+      </c>
+      <c r="C93">
+        <v>1739</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="F93" s="3">
+        <v>11</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B94">
+        <v>5</v>
+      </c>
+      <c r="C94">
+        <v>4149</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="2">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="F94" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="G94" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add first day of third round of measurements
</commit_message>
<xml_diff>
--- a/data_log_sheets/TT24_curve_log.xlsx
+++ b/data_log_sheets/TT24_curve_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data_log_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BA6651-42FD-DF4C-BB07-2D6A4838548A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01665EBA-1CE7-8D4D-8B16-32CF298A8220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="500" windowWidth="41420" windowHeight="28300" xr2:uid="{A62C6EB1-ACA7-F14B-BE94-73C128140FF4}"/>
+    <workbookView xWindow="9040" yWindow="500" windowWidth="42680" windowHeight="28300" xr2:uid="{A62C6EB1-ACA7-F14B-BE94-73C128140FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="62">
   <si>
     <t>date</t>
   </si>
@@ -204,6 +204,24 @@
   </si>
   <si>
     <t>4216 in log file</t>
+  </si>
+  <si>
+    <t>not including in analyses because it is in middle of garlic mustard path and on weeded side of plot. Inaccessible</t>
+  </si>
+  <si>
+    <t>browning leaves, not looking in great health</t>
+  </si>
+  <si>
+    <t>TT24_112</t>
+  </si>
+  <si>
+    <t>TT24_212</t>
+  </si>
+  <si>
+    <t>TT24_210</t>
+  </si>
+  <si>
+    <t>senesced</t>
   </si>
 </sst>
 </file>
@@ -581,11 +599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD84A7C-B77D-134C-A552-72D1D4E0C426}">
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="286" zoomScaleNormal="286" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F140" sqref="F140:G143"/>
+      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G288" sqref="G288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2451,7 +2469,7 @@
         <v>8</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -2477,7 +2495,7 @@
         <v>8</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -2503,7 +2521,7 @@
         <v>8</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -2529,7 +2547,7 @@
         <v>8</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -2555,7 +2573,7 @@
         <v>8</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -2581,7 +2599,7 @@
         <v>8</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -2607,7 +2625,7 @@
         <v>8</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -2633,7 +2651,7 @@
         <v>8</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -2659,7 +2677,7 @@
         <v>8</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -2685,7 +2703,7 @@
         <v>8</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -2711,7 +2729,7 @@
         <v>8</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2737,7 +2755,7 @@
         <v>8</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2763,7 +2781,7 @@
         <v>8</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2789,7 +2807,7 @@
         <v>8</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2815,7 +2833,7 @@
         <v>8</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2841,7 +2859,7 @@
         <v>8</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2867,7 +2885,7 @@
         <v>8</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2893,7 +2911,7 @@
         <v>8</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2919,7 +2937,7 @@
         <v>8</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2945,7 +2963,7 @@
         <v>8</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2971,7 +2989,7 @@
         <v>8</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2997,7 +3015,7 @@
         <v>8</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -3023,7 +3041,7 @@
         <v>8</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -4264,6 +4282,12 @@
       <c r="E140" s="2">
         <v>0.42152777777777778</v>
       </c>
+      <c r="F140" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G140" s="3">
+        <v>54.9</v>
+      </c>
       <c r="H140" s="3" t="s">
         <v>24</v>
       </c>
@@ -4284,6 +4308,12 @@
       <c r="E141" s="2">
         <v>0.43125000000000002</v>
       </c>
+      <c r="F141" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="G141" s="3">
+        <v>40.799999999999997</v>
+      </c>
       <c r="H141" s="3" t="s">
         <v>24</v>
       </c>
@@ -4304,6 +4334,12 @@
       <c r="E142" s="2">
         <v>0.44236111111111109</v>
       </c>
+      <c r="F142" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="G142" s="3">
+        <v>49.4</v>
+      </c>
       <c r="H142" s="3" t="s">
         <v>24</v>
       </c>
@@ -4324,6 +4360,12 @@
       <c r="E143" s="2">
         <v>0.45277777777777778</v>
       </c>
+      <c r="F143" s="3">
+        <v>21.1</v>
+      </c>
+      <c r="G143" s="3">
+        <v>74</v>
+      </c>
       <c r="H143" s="3" t="s">
         <v>24</v>
       </c>
@@ -4815,6 +4857,12 @@
       <c r="E162" s="2">
         <v>0.59791666666666665</v>
       </c>
+      <c r="F162" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="G162" s="3">
+        <v>41.5</v>
+      </c>
       <c r="H162" s="3" t="s">
         <v>24</v>
       </c>
@@ -4835,6 +4883,12 @@
       <c r="E163" s="2">
         <v>0.625</v>
       </c>
+      <c r="F163" s="3">
+        <v>17</v>
+      </c>
+      <c r="G163" s="3">
+        <v>80.099999999999994</v>
+      </c>
       <c r="H163" s="3" t="s">
         <v>24</v>
       </c>
@@ -5326,6 +5380,12 @@
       <c r="E182" s="2">
         <v>0.41458333333333336</v>
       </c>
+      <c r="F182" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="G182" s="3">
+        <v>67.2</v>
+      </c>
       <c r="H182" s="3" t="s">
         <v>24</v>
       </c>
@@ -5398,6 +5458,12 @@
       <c r="E185" s="2">
         <v>0.43194444444444446</v>
       </c>
+      <c r="F185" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="G185" s="3">
+        <v>54.3</v>
+      </c>
       <c r="H185" s="3" t="s">
         <v>24</v>
       </c>
@@ -5444,6 +5510,12 @@
       <c r="E187" s="2">
         <v>0.50763888888888886</v>
       </c>
+      <c r="F187" s="3">
+        <v>34.5</v>
+      </c>
+      <c r="G187" s="3">
+        <v>13.8</v>
+      </c>
       <c r="H187" s="3" t="s">
         <v>24</v>
       </c>
@@ -5464,6 +5536,12 @@
       <c r="E188" s="2">
         <v>0.44305555555555554</v>
       </c>
+      <c r="F188" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="G188" s="3">
+        <v>50.6</v>
+      </c>
       <c r="H188" s="3" t="s">
         <v>24</v>
       </c>
@@ -6906,6 +6984,1286 @@
         <v>8</v>
       </c>
       <c r="H244" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B245">
+        <v>5</v>
+      </c>
+      <c r="C245">
+        <v>7120</v>
+      </c>
+      <c r="D245" t="s">
+        <v>6</v>
+      </c>
+      <c r="E245" s="2">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="F245" s="3">
+        <v>14</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H245" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B246">
+        <v>5</v>
+      </c>
+      <c r="C246">
+        <v>2803</v>
+      </c>
+      <c r="D246" t="s">
+        <v>32</v>
+      </c>
+      <c r="E246" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="F246" s="3">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G246" s="3">
+        <v>51.9</v>
+      </c>
+      <c r="H246" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B247">
+        <v>5</v>
+      </c>
+      <c r="C247">
+        <v>1499</v>
+      </c>
+      <c r="D247" t="s">
+        <v>32</v>
+      </c>
+      <c r="E247" s="2">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="F247" s="3">
+        <v>19.2</v>
+      </c>
+      <c r="G247" s="3">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="H247" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B248">
+        <v>5</v>
+      </c>
+      <c r="C248">
+        <v>1432</v>
+      </c>
+      <c r="D248" t="s">
+        <v>32</v>
+      </c>
+      <c r="E248" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="F248" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G248" s="3">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="H248" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B249">
+        <v>5</v>
+      </c>
+      <c r="C249">
+        <v>2912</v>
+      </c>
+      <c r="D249" t="s">
+        <v>6</v>
+      </c>
+      <c r="E249" s="2">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="F249" s="3">
+        <v>15.7</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H249" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B250">
+        <v>5</v>
+      </c>
+      <c r="C250">
+        <v>614</v>
+      </c>
+      <c r="D250" t="s">
+        <v>6</v>
+      </c>
+      <c r="E250" s="2">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="F250" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="G250" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H250" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B251">
+        <v>5</v>
+      </c>
+      <c r="C251">
+        <v>6881</v>
+      </c>
+      <c r="D251" t="s">
+        <v>6</v>
+      </c>
+      <c r="E251" s="2">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="F251" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="G251" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H251" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B252">
+        <v>5</v>
+      </c>
+      <c r="C252">
+        <v>1374</v>
+      </c>
+      <c r="D252" t="s">
+        <v>6</v>
+      </c>
+      <c r="E252" s="2">
+        <v>0.51527777777777772</v>
+      </c>
+      <c r="F252" s="3">
+        <v>14.3</v>
+      </c>
+      <c r="G252" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H252" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B253">
+        <v>5</v>
+      </c>
+      <c r="C253">
+        <v>1826</v>
+      </c>
+      <c r="D253" t="s">
+        <v>6</v>
+      </c>
+      <c r="E253" s="2">
+        <v>0.52847222222222223</v>
+      </c>
+      <c r="F253" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G253" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H253" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A254" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B254">
+        <v>5</v>
+      </c>
+      <c r="C254">
+        <v>4105</v>
+      </c>
+      <c r="D254" t="s">
+        <v>6</v>
+      </c>
+      <c r="E254" s="2">
+        <v>0.54236111111111107</v>
+      </c>
+      <c r="F254" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="G254" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H254" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A255" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B255">
+        <v>5</v>
+      </c>
+      <c r="C255">
+        <v>5381</v>
+      </c>
+      <c r="D255" t="s">
+        <v>6</v>
+      </c>
+      <c r="E255" s="2">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="F255" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G255" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H255" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A256" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B256">
+        <v>5</v>
+      </c>
+      <c r="C256">
+        <v>4574</v>
+      </c>
+      <c r="D256" t="s">
+        <v>6</v>
+      </c>
+      <c r="E256" s="2">
+        <v>0.51458333333333328</v>
+      </c>
+      <c r="F256" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="G256" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H256" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A257" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B257">
+        <v>5</v>
+      </c>
+      <c r="C257" t="s">
+        <v>22</v>
+      </c>
+      <c r="D257" t="s">
+        <v>6</v>
+      </c>
+      <c r="E257" s="2">
+        <v>0.58402777777777781</v>
+      </c>
+      <c r="F257" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="G257" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H257" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A258" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B258">
+        <v>5</v>
+      </c>
+      <c r="C258">
+        <v>2563</v>
+      </c>
+      <c r="D258" t="s">
+        <v>6</v>
+      </c>
+      <c r="E258" s="2">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="F258" s="3">
+        <v>19.3</v>
+      </c>
+      <c r="G258" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H258" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A259" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B259">
+        <v>5</v>
+      </c>
+      <c r="C259">
+        <v>4177</v>
+      </c>
+      <c r="D259" t="s">
+        <v>6</v>
+      </c>
+      <c r="E259" s="2">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="F259" s="3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G259" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H259" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A260" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B260">
+        <v>5</v>
+      </c>
+      <c r="C260">
+        <v>3</v>
+      </c>
+      <c r="D260" t="s">
+        <v>6</v>
+      </c>
+      <c r="E260" t="s">
+        <v>8</v>
+      </c>
+      <c r="F260" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="G260" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H260" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A261" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B261">
+        <v>5</v>
+      </c>
+      <c r="C261">
+        <v>1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>6</v>
+      </c>
+      <c r="E261" s="2">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="F261" s="3">
+        <v>12</v>
+      </c>
+      <c r="G261" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H261" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I261" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B262">
+        <v>5</v>
+      </c>
+      <c r="C262">
+        <v>2</v>
+      </c>
+      <c r="D262" t="s">
+        <v>6</v>
+      </c>
+      <c r="E262" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="F262" s="3">
+        <v>16.8</v>
+      </c>
+      <c r="G262" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H262" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B263">
+        <v>5</v>
+      </c>
+      <c r="C263">
+        <v>4149</v>
+      </c>
+      <c r="D263" t="s">
+        <v>6</v>
+      </c>
+      <c r="E263" s="2">
+        <v>0.47361111111111109</v>
+      </c>
+      <c r="F263" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="G263" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H263" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B264">
+        <v>5</v>
+      </c>
+      <c r="C264">
+        <v>1795</v>
+      </c>
+      <c r="D264" t="s">
+        <v>6</v>
+      </c>
+      <c r="E264" s="2">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="F264" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="G264" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H264" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B265">
+        <v>5</v>
+      </c>
+      <c r="C265">
+        <v>6887</v>
+      </c>
+      <c r="D265" t="s">
+        <v>6</v>
+      </c>
+      <c r="E265" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F265" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="G265" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H265" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B266">
+        <v>5</v>
+      </c>
+      <c r="C266">
+        <v>2</v>
+      </c>
+      <c r="D266" t="s">
+        <v>32</v>
+      </c>
+      <c r="E266" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="F266" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="G266" s="3">
+        <v>28.1</v>
+      </c>
+      <c r="H266" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B267">
+        <v>5</v>
+      </c>
+      <c r="C267">
+        <v>631</v>
+      </c>
+      <c r="D267" t="s">
+        <v>32</v>
+      </c>
+      <c r="E267" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="F267" s="3">
+        <v>17</v>
+      </c>
+      <c r="G267" s="3">
+        <v>59</v>
+      </c>
+      <c r="H267" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B268">
+        <v>5</v>
+      </c>
+      <c r="C268">
+        <v>3960</v>
+      </c>
+      <c r="D268" t="s">
+        <v>32</v>
+      </c>
+      <c r="E268" s="2">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="F268" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G268" s="3">
+        <v>52</v>
+      </c>
+      <c r="H268" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B269">
+        <v>5</v>
+      </c>
+      <c r="C269">
+        <v>3993</v>
+      </c>
+      <c r="D269" t="s">
+        <v>32</v>
+      </c>
+      <c r="E269" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="F269" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="G269" s="3">
+        <v>45.1</v>
+      </c>
+      <c r="H269" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B270">
+        <v>5</v>
+      </c>
+      <c r="C270">
+        <v>86</v>
+      </c>
+      <c r="D270" t="s">
+        <v>6</v>
+      </c>
+      <c r="E270" s="2">
+        <v>0.56736111111111109</v>
+      </c>
+      <c r="F270" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="G270" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H270" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B271">
+        <v>5</v>
+      </c>
+      <c r="C271">
+        <v>7147</v>
+      </c>
+      <c r="D271" t="s">
+        <v>6</v>
+      </c>
+      <c r="E271" s="2">
+        <v>0.57638888888888884</v>
+      </c>
+      <c r="F271" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="G271" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H271" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B272">
+        <v>5</v>
+      </c>
+      <c r="C272">
+        <v>43</v>
+      </c>
+      <c r="D272" t="s">
+        <v>6</v>
+      </c>
+      <c r="E272" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="F272" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="G272" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H272" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B273">
+        <v>5</v>
+      </c>
+      <c r="C273">
+        <v>5904</v>
+      </c>
+      <c r="D273" t="s">
+        <v>6</v>
+      </c>
+      <c r="E273" t="s">
+        <v>8</v>
+      </c>
+      <c r="F273" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G273" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H273" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I273" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B274">
+        <v>3</v>
+      </c>
+      <c r="C274">
+        <v>4250</v>
+      </c>
+      <c r="D274" t="s">
+        <v>32</v>
+      </c>
+      <c r="E274" s="2">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="F274" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="G274" s="3">
+        <v>29.8</v>
+      </c>
+      <c r="H274" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B275">
+        <v>3</v>
+      </c>
+      <c r="C275" t="s">
+        <v>58</v>
+      </c>
+      <c r="D275" t="s">
+        <v>32</v>
+      </c>
+      <c r="E275" s="2">
+        <v>0.43402777777777779</v>
+      </c>
+      <c r="F275" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="G275" s="3">
+        <v>54</v>
+      </c>
+      <c r="H275" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B276">
+        <v>3</v>
+      </c>
+      <c r="C276">
+        <v>5436</v>
+      </c>
+      <c r="D276" t="s">
+        <v>6</v>
+      </c>
+      <c r="E276" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F276" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G276" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H276" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B277">
+        <v>3</v>
+      </c>
+      <c r="C277">
+        <v>9412</v>
+      </c>
+      <c r="D277" t="s">
+        <v>32</v>
+      </c>
+      <c r="E277" s="2">
+        <v>0.46527777777777779</v>
+      </c>
+      <c r="F277" s="3">
+        <v>15.6</v>
+      </c>
+      <c r="G277" s="3">
+        <v>45.9</v>
+      </c>
+      <c r="H277" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B278">
+        <v>3</v>
+      </c>
+      <c r="C278">
+        <v>5495</v>
+      </c>
+      <c r="D278" t="s">
+        <v>6</v>
+      </c>
+      <c r="E278" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F278" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="G278" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H278" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B279">
+        <v>3</v>
+      </c>
+      <c r="C279">
+        <v>3563</v>
+      </c>
+      <c r="D279" t="s">
+        <v>6</v>
+      </c>
+      <c r="E279" s="2">
+        <v>0.49930555555555556</v>
+      </c>
+      <c r="F279" s="3">
+        <v>9.9</v>
+      </c>
+      <c r="G279" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H279" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B280">
+        <v>3</v>
+      </c>
+      <c r="C280" t="s">
+        <v>59</v>
+      </c>
+      <c r="D280" t="s">
+        <v>32</v>
+      </c>
+      <c r="E280" s="2">
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="F280" s="3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G280" s="3">
+        <v>52.7</v>
+      </c>
+      <c r="H280" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B281">
+        <v>3</v>
+      </c>
+      <c r="C281">
+        <v>2310</v>
+      </c>
+      <c r="D281" t="s">
+        <v>32</v>
+      </c>
+      <c r="E281" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="F281" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="G281" s="3">
+        <v>33.9</v>
+      </c>
+      <c r="H281" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B282">
+        <v>3</v>
+      </c>
+      <c r="C282" t="s">
+        <v>60</v>
+      </c>
+      <c r="D282" t="s">
+        <v>32</v>
+      </c>
+      <c r="E282" s="2">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="F282" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="G282" s="3">
+        <v>51.8</v>
+      </c>
+      <c r="H282" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B283">
+        <v>3</v>
+      </c>
+      <c r="C283">
+        <v>1686</v>
+      </c>
+      <c r="D283" t="s">
+        <v>6</v>
+      </c>
+      <c r="E283" s="2">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="F283" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G283" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H283" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B284">
+        <v>3</v>
+      </c>
+      <c r="C284">
+        <v>5797</v>
+      </c>
+      <c r="D284" t="s">
+        <v>6</v>
+      </c>
+      <c r="E284" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F284" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="G284" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H284" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B285">
+        <v>3</v>
+      </c>
+      <c r="C285">
+        <v>4714</v>
+      </c>
+      <c r="D285" t="s">
+        <v>6</v>
+      </c>
+      <c r="E285" s="2">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="F285" s="3">
+        <v>11</v>
+      </c>
+      <c r="H285" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B286">
+        <v>3</v>
+      </c>
+      <c r="C286">
+        <v>902</v>
+      </c>
+      <c r="D286" t="s">
+        <v>6</v>
+      </c>
+      <c r="E286" t="s">
+        <v>8</v>
+      </c>
+      <c r="F286" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G286" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H286" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I286" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B287">
+        <v>3</v>
+      </c>
+      <c r="C287">
+        <v>5105</v>
+      </c>
+      <c r="D287" t="s">
+        <v>32</v>
+      </c>
+      <c r="E287" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F287" s="3">
+        <v>14</v>
+      </c>
+      <c r="G287" s="3">
+        <v>34</v>
+      </c>
+      <c r="H287" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B288">
+        <v>3</v>
+      </c>
+      <c r="C288">
+        <v>2329</v>
+      </c>
+      <c r="D288" t="s">
+        <v>6</v>
+      </c>
+      <c r="E288" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="F288" s="3">
+        <v>13</v>
+      </c>
+      <c r="G288" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H288" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B289">
+        <v>3</v>
+      </c>
+      <c r="C289">
+        <v>6885</v>
+      </c>
+      <c r="D289" t="s">
+        <v>6</v>
+      </c>
+      <c r="E289" s="2">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="F289" s="3">
+        <v>12</v>
+      </c>
+      <c r="G289" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H289" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B290">
+        <v>3</v>
+      </c>
+      <c r="C290">
+        <v>774</v>
+      </c>
+      <c r="D290" t="s">
+        <v>6</v>
+      </c>
+      <c r="E290" s="2">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="F290" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="G290" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H290" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B291">
+        <v>3</v>
+      </c>
+      <c r="C291">
+        <v>5184</v>
+      </c>
+      <c r="D291" t="s">
+        <v>32</v>
+      </c>
+      <c r="E291" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F291" s="3">
+        <v>16</v>
+      </c>
+      <c r="G291" s="3">
+        <v>34.5</v>
+      </c>
+      <c r="H291" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B292">
+        <v>3</v>
+      </c>
+      <c r="C292">
+        <v>141</v>
+      </c>
+      <c r="D292" t="s">
+        <v>32</v>
+      </c>
+      <c r="E292" s="2">
+        <v>0.46944444444444444</v>
+      </c>
+      <c r="F292" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="G292" s="3">
+        <v>41</v>
+      </c>
+      <c r="H292" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B293">
+        <v>3</v>
+      </c>
+      <c r="C293">
+        <v>552</v>
+      </c>
+      <c r="D293" t="s">
+        <v>6</v>
+      </c>
+      <c r="E293" s="2">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="F293" s="3">
+        <v>13</v>
+      </c>
+      <c r="G293" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H293" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
continue fitting curves. halfway point
</commit_message>
<xml_diff>
--- a/data_log_sheets/TT24_curve_log.xlsx
+++ b/data_log_sheets/TT24_curve_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data_log_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A34FD71-A771-B34F-81A0-D6BDCCA46696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BE7D87-3D5A-FA4F-B1B1-17C94F64F8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{D520579F-2F6B-D846-98D0-14D12C1E8BAA}"/>
   </bookViews>
@@ -772,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -793,15 +793,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1521,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2542542-07FB-D144-949C-9817BEAE737F}">
   <dimension ref="A1:K936"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="I388" sqref="I388"/>
+    <sheetView tabSelected="1" topLeftCell="A475" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="I479" sqref="I479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12601,26 +12592,26 @@
       <c r="C355" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D355" s="8">
+      <c r="D355" s="4">
         <v>4109</v>
       </c>
-      <c r="E355" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F355" s="9">
+      <c r="E355" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F355" s="5">
         <v>0.56944444444444442</v>
       </c>
-      <c r="G355" s="10">
+      <c r="G355" s="6">
         <v>12.7</v>
       </c>
-      <c r="H355" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I355" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J355" s="8"/>
-      <c r="K355" s="10"/>
+      <c r="H355" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I355" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J355" s="4"/>
+      <c r="K355" s="6"/>
     </row>
     <row r="356" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A356" s="3">
@@ -13652,7 +13643,7 @@
         <v>54.2</v>
       </c>
       <c r="I388" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J388" s="4"/>
       <c r="K388" s="6"/>
@@ -13683,7 +13674,7 @@
         <v>41.8</v>
       </c>
       <c r="I389" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J389" s="4"/>
       <c r="K389" s="6"/>
@@ -13714,7 +13705,7 @@
         <v>57.2</v>
       </c>
       <c r="I390" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J390" s="4"/>
       <c r="K390" s="6"/>
@@ -13745,7 +13736,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="I391" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J391" s="4"/>
       <c r="K391" s="6"/>
@@ -13776,7 +13767,7 @@
         <v>32.5</v>
       </c>
       <c r="I392" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J392" s="4"/>
       <c r="K392" s="6"/>
@@ -13807,7 +13798,7 @@
         <v>57.9</v>
       </c>
       <c r="I393" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J393" s="4"/>
       <c r="K393" s="6"/>
@@ -13838,7 +13829,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="I394" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J394" s="4"/>
       <c r="K394" s="6"/>
@@ -13869,7 +13860,7 @@
         <v>73.400000000000006</v>
       </c>
       <c r="I395" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J395" s="4"/>
       <c r="K395" s="6"/>
@@ -13900,7 +13891,7 @@
         <v>10</v>
       </c>
       <c r="I396" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J396" s="4" t="s">
         <v>212</v>
@@ -13933,7 +13924,7 @@
         <v>56.9</v>
       </c>
       <c r="I397" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J397" s="4"/>
       <c r="K397" s="6"/>
@@ -13964,7 +13955,7 @@
         <v>10</v>
       </c>
       <c r="I398" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J398" s="4"/>
       <c r="K398" s="6"/>
@@ -13995,7 +13986,7 @@
         <v>10</v>
       </c>
       <c r="I399" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J399" s="4"/>
       <c r="K399" s="6"/>
@@ -14026,7 +14017,7 @@
         <v>10</v>
       </c>
       <c r="I400" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J400" s="4"/>
       <c r="K400" s="6"/>
@@ -14057,7 +14048,7 @@
         <v>10</v>
       </c>
       <c r="I401" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J401" s="4" t="s">
         <v>203</v>
@@ -14090,7 +14081,7 @@
         <v>37.299999999999997</v>
       </c>
       <c r="I402" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J402" s="4"/>
       <c r="K402" s="6"/>
@@ -14121,7 +14112,7 @@
         <v>49.5</v>
       </c>
       <c r="I403" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J403" s="4"/>
       <c r="K403" s="6"/>
@@ -14152,7 +14143,7 @@
         <v>10</v>
       </c>
       <c r="I404" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J404" s="4"/>
       <c r="K404" s="6"/>
@@ -14183,7 +14174,7 @@
         <v>62.2</v>
       </c>
       <c r="I405" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J405" s="4"/>
       <c r="K405" s="6"/>
@@ -14214,7 +14205,7 @@
         <v>46</v>
       </c>
       <c r="I406" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J406" s="4"/>
       <c r="K406" s="6"/>
@@ -14245,7 +14236,7 @@
         <v>61.5</v>
       </c>
       <c r="I407" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J407" s="4"/>
       <c r="K407" s="6"/>
@@ -14276,7 +14267,7 @@
         <v>63.5</v>
       </c>
       <c r="I408" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J408" s="4"/>
       <c r="K408" s="6"/>
@@ -14307,7 +14298,7 @@
         <v>59.6</v>
       </c>
       <c r="I409" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J409" s="4"/>
       <c r="K409" s="6"/>
@@ -14338,7 +14329,7 @@
         <v>28.5</v>
       </c>
       <c r="I410" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J410" s="4" t="s">
         <v>218</v>
@@ -14371,7 +14362,7 @@
         <v>10</v>
       </c>
       <c r="I411" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J411" s="4" t="s">
         <v>217</v>
@@ -14404,7 +14395,7 @@
         <v>10</v>
       </c>
       <c r="I412" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J412" s="4"/>
       <c r="K412" s="6"/>
@@ -14420,7 +14411,7 @@
         <v>209</v>
       </c>
       <c r="D413" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E413" s="4" t="s">
         <v>33</v>
@@ -14435,7 +14426,7 @@
         <v>45.6</v>
       </c>
       <c r="I413" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J413" s="4" t="s">
         <v>215</v>
@@ -14468,7 +14459,7 @@
         <v>10</v>
       </c>
       <c r="I414" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J414" s="4"/>
       <c r="K414" s="6"/>
@@ -14499,7 +14490,7 @@
         <v>10</v>
       </c>
       <c r="I415" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J415" s="4"/>
       <c r="K415" s="6"/>
@@ -14530,7 +14521,7 @@
         <v>10</v>
       </c>
       <c r="I416" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J416" s="4" t="s">
         <v>214</v>
@@ -14563,7 +14554,7 @@
         <v>10</v>
       </c>
       <c r="I417" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J417" s="4" t="s">
         <v>213</v>
@@ -14581,7 +14572,7 @@
         <v>209</v>
       </c>
       <c r="D418" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E418" s="4" t="s">
         <v>33</v>
@@ -14596,7 +14587,7 @@
         <v>39</v>
       </c>
       <c r="I418" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J418" s="4" t="s">
         <v>216</v>
@@ -14629,7 +14620,7 @@
         <v>10</v>
       </c>
       <c r="I419" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J419" s="4"/>
       <c r="K419" s="6"/>
@@ -14660,7 +14651,7 @@
         <v>10</v>
       </c>
       <c r="I420" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J420" s="4"/>
       <c r="K420" s="6"/>
@@ -14691,7 +14682,7 @@
         <v>10</v>
       </c>
       <c r="I421" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J421" s="4"/>
       <c r="K421" s="6"/>
@@ -14722,7 +14713,7 @@
         <v>10</v>
       </c>
       <c r="I422" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J422" s="4"/>
       <c r="K422" s="6"/>
@@ -14753,7 +14744,7 @@
         <v>10</v>
       </c>
       <c r="I423" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J423" s="4"/>
       <c r="K423" s="6"/>
@@ -14784,7 +14775,7 @@
         <v>10</v>
       </c>
       <c r="I424" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J424" s="4"/>
       <c r="K424" s="6"/>
@@ -14815,7 +14806,7 @@
         <v>61.5</v>
       </c>
       <c r="I425" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J425" s="4"/>
       <c r="K425" s="6"/>
@@ -14846,7 +14837,7 @@
         <v>58.1</v>
       </c>
       <c r="I426" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J426" s="4"/>
       <c r="K426" s="6"/>
@@ -14877,7 +14868,7 @@
         <v>27.3</v>
       </c>
       <c r="I427" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J427" s="4"/>
       <c r="K427" s="6"/>
@@ -14908,7 +14899,7 @@
         <v>66.099999999999994</v>
       </c>
       <c r="I428" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J428" s="4"/>
       <c r="K428" s="6"/>
@@ -14939,7 +14930,7 @@
         <v>10</v>
       </c>
       <c r="I429" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J429" s="4"/>
       <c r="K429" s="6"/>
@@ -14970,7 +14961,7 @@
         <v>10</v>
       </c>
       <c r="I430" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J430" s="4"/>
       <c r="K430" s="6"/>
@@ -15001,7 +14992,7 @@
         <v>10</v>
       </c>
       <c r="I431" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J431" s="4"/>
       <c r="K431" s="6"/>
@@ -15032,7 +15023,7 @@
         <v>10</v>
       </c>
       <c r="I432" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J432" s="4" t="s">
         <v>76</v>
@@ -15065,7 +15056,7 @@
         <v>10</v>
       </c>
       <c r="I433" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J433" s="4"/>
       <c r="K433" s="6"/>
@@ -15096,7 +15087,7 @@
         <v>10</v>
       </c>
       <c r="I434" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J434" s="4"/>
       <c r="K434" s="6"/>
@@ -15127,7 +15118,7 @@
         <v>10</v>
       </c>
       <c r="I435" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J435" s="4"/>
       <c r="K435" s="6"/>
@@ -15158,7 +15149,7 @@
         <v>18.2</v>
       </c>
       <c r="I436" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J436" s="4" t="s">
         <v>78</v>
@@ -15191,7 +15182,7 @@
         <v>15</v>
       </c>
       <c r="I437" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J437" s="4" t="s">
         <v>79</v>
@@ -15224,7 +15215,7 @@
         <v>56.9</v>
       </c>
       <c r="I438" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J438" s="4"/>
       <c r="K438" s="6"/>
@@ -15255,7 +15246,7 @@
         <v>63.6</v>
       </c>
       <c r="I439" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J439" s="4"/>
       <c r="K439" s="6"/>
@@ -15286,7 +15277,7 @@
         <v>72.900000000000006</v>
       </c>
       <c r="I440" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J440" s="4" t="s">
         <v>80</v>
@@ -15319,7 +15310,7 @@
         <v>79</v>
       </c>
       <c r="I441" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J441" s="4"/>
       <c r="K441" s="6"/>
@@ -15350,7 +15341,7 @@
         <v>52.6</v>
       </c>
       <c r="I442" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J442" s="4" t="s">
         <v>81</v>
@@ -15383,7 +15374,7 @@
         <v>10</v>
       </c>
       <c r="I443" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J443" s="4" t="s">
         <v>82</v>
@@ -15401,7 +15392,7 @@
         <v>209</v>
       </c>
       <c r="D444" s="4">
-        <v>4171</v>
+        <v>4177</v>
       </c>
       <c r="E444" s="4" t="s">
         <v>9</v>
@@ -15416,7 +15407,7 @@
         <v>10</v>
       </c>
       <c r="I444" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J444" s="4" t="s">
         <v>83</v>
@@ -15449,7 +15440,7 @@
         <v>10</v>
       </c>
       <c r="I445" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J445" s="4" t="s">
         <v>83</v>
@@ -15482,7 +15473,7 @@
         <v>10</v>
       </c>
       <c r="I446" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J446" s="4" t="s">
         <v>83</v>
@@ -15515,7 +15506,7 @@
         <v>10</v>
       </c>
       <c r="I447" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J447" s="4"/>
       <c r="K447" s="6"/>
@@ -15546,7 +15537,7 @@
         <v>10</v>
       </c>
       <c r="I448" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J448" s="4"/>
       <c r="K448" s="6"/>
@@ -15577,7 +15568,7 @@
         <v>61.1</v>
       </c>
       <c r="I449" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J449" s="4"/>
       <c r="K449" s="6"/>
@@ -15608,7 +15599,7 @@
         <v>31.2</v>
       </c>
       <c r="I450" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J450" s="4"/>
       <c r="K450" s="6"/>
@@ -15639,7 +15630,7 @@
         <v>53.3</v>
       </c>
       <c r="I451" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J451" s="4"/>
       <c r="K451" s="6"/>
@@ -15670,7 +15661,7 @@
         <v>44.5</v>
       </c>
       <c r="I452" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J452" s="4"/>
       <c r="K452" s="6"/>
@@ -15701,7 +15692,7 @@
         <v>43.6</v>
       </c>
       <c r="I453" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J453" s="4"/>
       <c r="K453" s="6"/>
@@ -15732,7 +15723,7 @@
         <v>42.3</v>
       </c>
       <c r="I454" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J454" s="4"/>
       <c r="K454" s="6"/>
@@ -15763,7 +15754,7 @@
         <v>10</v>
       </c>
       <c r="I455" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J455" s="4"/>
       <c r="K455" s="6"/>
@@ -15794,7 +15785,7 @@
         <v>40.4</v>
       </c>
       <c r="I456" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J456" s="4"/>
       <c r="K456" s="6"/>
@@ -15825,7 +15816,7 @@
         <v>53.5</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J457" s="4"/>
       <c r="K457" s="6"/>
@@ -15856,7 +15847,7 @@
         <v>52.8</v>
       </c>
       <c r="I458" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J458" s="4"/>
       <c r="K458" s="6"/>
@@ -15887,7 +15878,7 @@
         <v>10</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J459" s="4" t="s">
         <v>86</v>
@@ -15920,7 +15911,7 @@
         <v>10</v>
       </c>
       <c r="I460" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J460" s="4" t="s">
         <v>87</v>
@@ -15953,7 +15944,7 @@
         <v>10</v>
       </c>
       <c r="I461" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J461" s="4"/>
       <c r="K461" s="6"/>
@@ -15984,7 +15975,7 @@
         <v>10</v>
       </c>
       <c r="I462" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J462" s="4"/>
       <c r="K462" s="6"/>
@@ -16015,7 +16006,7 @@
         <v>10</v>
       </c>
       <c r="I463" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J463" s="4"/>
       <c r="K463" s="6"/>
@@ -16046,7 +16037,7 @@
         <v>20.5</v>
       </c>
       <c r="I464" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J464" s="4"/>
       <c r="K464" s="6"/>
@@ -16077,7 +16068,7 @@
         <v>34.799999999999997</v>
       </c>
       <c r="I465" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J465" s="4"/>
       <c r="K465" s="6"/>
@@ -16108,7 +16099,7 @@
         <v>64.3</v>
       </c>
       <c r="I466" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J466" s="4" t="s">
         <v>88</v>
@@ -16141,7 +16132,7 @@
         <v>53.5</v>
       </c>
       <c r="I467" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J467" s="4" t="s">
         <v>89</v>
@@ -16174,7 +16165,7 @@
         <v>39.200000000000003</v>
       </c>
       <c r="I468" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J468" s="4" t="s">
         <v>90</v>
@@ -16207,7 +16198,7 @@
         <v>39.700000000000003</v>
       </c>
       <c r="I469" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J469" s="4" t="s">
         <v>91</v>
@@ -16240,7 +16231,7 @@
         <v>24.2</v>
       </c>
       <c r="I470" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J470" s="4" t="s">
         <v>91</v>
@@ -16273,7 +16264,7 @@
         <v>15.9</v>
       </c>
       <c r="I471" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J471" s="4" t="s">
         <v>92</v>
@@ -16306,7 +16297,7 @@
         <v>58.8</v>
       </c>
       <c r="I472" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J472" s="4" t="s">
         <v>93</v>
@@ -16339,7 +16330,7 @@
         <v>25.9</v>
       </c>
       <c r="I473" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J473" s="4"/>
       <c r="K473" s="6"/>
@@ -16370,7 +16361,7 @@
         <v>10</v>
       </c>
       <c r="I474" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J474" s="4"/>
       <c r="K474" s="6"/>
@@ -16401,7 +16392,7 @@
         <v>58.2</v>
       </c>
       <c r="I475" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J475" s="4" t="s">
         <v>94</v>
@@ -16434,7 +16425,7 @@
         <v>37.700000000000003</v>
       </c>
       <c r="I476" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J476" s="4"/>
       <c r="K476" s="6"/>
@@ -16465,7 +16456,7 @@
         <v>10</v>
       </c>
       <c r="I477" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J477" s="4"/>
       <c r="K477" s="6"/>
@@ -16496,7 +16487,7 @@
         <v>46.1</v>
       </c>
       <c r="I478" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J478" s="4"/>
       <c r="K478" s="6"/>

</xml_diff>